<commit_message>
final commit -all test cases are coverd, with base classes inheritance
</commit_message>
<xml_diff>
--- a/files/conduittests/login/LoginWithInvalidCredentialsTest.xlsx
+++ b/files/conduittests/login/LoginWithInvalidCredentialsTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesamM\Desktop\automation-project\files\conduittests\login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93394D87-615A-4134-B7A9-0577A6749DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F3861C-1835-492C-A039-5D22FAE87EBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4365" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{E364FD4F-E7B1-41D7-962F-328A4F9F0024}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Run</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>1234567</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>test case number 5</t>
+  </si>
+  <si>
+    <t>dummy</t>
   </si>
 </sst>
 </file>
@@ -447,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C28D33-4FEE-4249-85B6-B425EED4424F}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +526,7 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>10</v>
@@ -533,8 +545,8 @@
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1">
-        <v>123456789</v>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
@@ -553,6 +565,26 @@
       <c r="D5" s="2"/>
       <c r="E5" s="1"/>
       <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>